<commit_message>
Reworked how inventory, look at, and take function
</commit_message>
<xml_diff>
--- a/TextGame_RoomLayout.xlsx
+++ b/TextGame_RoomLayout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Python37\Projects\TextGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{58FA33B0-B351-41DD-90DE-1EDC7D954317}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C12EF7B-666E-4548-B1C8-AE8234C52E8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12108" yWindow="-8172" windowWidth="17280" windowHeight="8964" xr2:uid="{EA67EDC3-4EE7-4B5B-990C-81672A58C201}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EA67EDC3-4EE7-4B5B-990C-81672A58C201}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,8 +51,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -68,7 +76,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -91,13 +99,290 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,139 +700,139 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:F10"/>
+      <selection activeCell="D11" sqref="D11:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="A1" s="24"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="5"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="7"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="7"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="10"/>
+    </row>
+    <row r="6" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
+      <c r="B6" s="22"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1" t="s">
+      <c r="E6" s="22"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="7"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="7"/>
+    </row>
+    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="15"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>

</xml_diff>

<commit_message>
Added items/room ; will modify money and players next
</commit_message>
<xml_diff>
--- a/TextGame_RoomLayout.xlsx
+++ b/TextGame_RoomLayout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Python37\Projects\TextGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C12EF7B-666E-4548-B1C8-AE8234C52E8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62950962-AC82-4940-978F-ACA9AF9EBE89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EA67EDC3-4EE7-4B5B-990C-81672A58C201}"/>
+    <workbookView xWindow="6408" yWindow="-15948" windowWidth="19572" windowHeight="13884" xr2:uid="{EA67EDC3-4EE7-4B5B-990C-81672A58C201}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Kitchen</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Dining Hall to Ballroom Hallway</t>
+  </si>
+  <si>
+    <t>Living Room</t>
   </si>
 </sst>
 </file>
@@ -76,7 +79,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -233,45 +236,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -301,86 +265,103 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -697,189 +678,207 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7668094A-7216-4F66-81FF-EE21FC4176DC}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:F15"/>
+      <selection activeCell="G11" sqref="G11:I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="24"/>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="18" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="12"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="5"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="7"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="7"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="7"/>
-    </row>
-    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="25"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="10"/>
-    </row>
-    <row r="6" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="21" t="s">
+      <c r="H1" s="13"/>
+      <c r="I1" s="14"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="16"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="16"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="16"/>
+    </row>
+    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="18"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="21" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="11" t="s">
+      <c r="E6" s="4"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="7"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="7"/>
-    </row>
-    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="15"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="10"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="13"/>
+      <c r="L6" s="14"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="16"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="16"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="16"/>
+    </row>
+    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="18"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="J6:L10"/>
     <mergeCell ref="A11:C15"/>
     <mergeCell ref="D11:F15"/>
     <mergeCell ref="G11:I15"/>

</xml_diff>

<commit_message>
++foyer, upstairs hallway, items, keys  -- living room.
</commit_message>
<xml_diff>
--- a/TextGame_RoomLayout.xlsx
+++ b/TextGame_RoomLayout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Python37\Projects\TextGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62950962-AC82-4940-978F-ACA9AF9EBE89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{668E3F95-DF22-41D2-8CF0-ED7981F46D86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6408" yWindow="-15948" windowWidth="19572" windowHeight="13884" xr2:uid="{EA67EDC3-4EE7-4B5B-990C-81672A58C201}"/>
+    <workbookView xWindow="12912" yWindow="0" windowWidth="10128" windowHeight="12204" xr2:uid="{EA67EDC3-4EE7-4B5B-990C-81672A58C201}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Kitchen</t>
   </si>
@@ -47,7 +47,13 @@
     <t>Dining Hall to Ballroom Hallway</t>
   </si>
   <si>
-    <t>Living Room</t>
+    <t>Study</t>
+  </si>
+  <si>
+    <t>Upstairs Hallway</t>
+  </si>
+  <si>
+    <t>Foyer</t>
   </si>
 </sst>
 </file>
@@ -296,6 +302,33 @@
   </cellStyleXfs>
   <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -326,33 +359,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -681,56 +687,56 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11:I15"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="12"/>
-      <c r="B1" s="12"/>
+      <c r="A1" s="21"/>
+      <c r="B1" s="21"/>
       <c r="C1" s="23"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="19" t="s">
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="13"/>
-      <c r="I1" s="14"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="3"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
       <c r="C2" s="23"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="16"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
       <c r="C3" s="23"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="16"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
       <c r="C4" s="23"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="16"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22"/>
@@ -739,155 +745,175 @@
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
       <c r="F5" s="22"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="18"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="9"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="3" t="s">
+      <c r="B6" s="13"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="19" t="s">
+      <c r="E6" s="13"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="19" t="s">
+      <c r="H6" s="2"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="13"/>
-      <c r="L6" s="14"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="3"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="16"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="6"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="16"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="6"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="16"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="6"/>
     </row>
     <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="18"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="9"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K11" s="2"/>
+      <c r="L11" s="3"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="6"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="6"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="6"/>
+    </row>
+    <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="J11:L15"/>
+    <mergeCell ref="D1:F5"/>
+    <mergeCell ref="A1:C5"/>
+    <mergeCell ref="A6:C10"/>
+    <mergeCell ref="G1:I5"/>
+    <mergeCell ref="G6:I10"/>
     <mergeCell ref="J6:L10"/>
     <mergeCell ref="A11:C15"/>
     <mergeCell ref="D11:F15"/>
     <mergeCell ref="G11:I15"/>
     <mergeCell ref="D6:F10"/>
-    <mergeCell ref="D1:F5"/>
-    <mergeCell ref="A1:C5"/>
-    <mergeCell ref="A6:C10"/>
-    <mergeCell ref="G1:I5"/>
-    <mergeCell ref="G6:I10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed fight and insult (I think) and ++ br & sword
</commit_message>
<xml_diff>
--- a/TextGame_RoomLayout.xlsx
+++ b/TextGame_RoomLayout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Python37\Projects\TextGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{668E3F95-DF22-41D2-8CF0-ED7981F46D86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD7D057-D9B1-40DA-983E-13B74C04C3A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12912" yWindow="0" windowWidth="10128" windowHeight="12204" xr2:uid="{EA67EDC3-4EE7-4B5B-990C-81672A58C201}"/>
+    <workbookView xWindow="-3924" yWindow="-13620" windowWidth="19704" windowHeight="12396" xr2:uid="{EA67EDC3-4EE7-4B5B-990C-81672A58C201}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Kitchen</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Foyer</t>
+  </si>
+  <si>
+    <t>Bedroom</t>
   </si>
 </sst>
 </file>
@@ -329,47 +332,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -684,82 +687,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7668094A-7216-4F66-81FF-EE21FC4176DC}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="21"/>
-      <c r="B1" s="21"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="10"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
       <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="3"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
       <c r="G3" s="4"/>
       <c r="H3" s="5"/>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="21"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
       <c r="G4" s="4"/>
       <c r="H4" s="5"/>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
+    <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
       <c r="G5" s="7"/>
       <c r="H5" s="8"/>
       <c r="I5" s="9"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="12" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="14"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="16"/>
       <c r="G6" s="1" t="s">
         <v>1</v>
       </c>
@@ -771,13 +774,13 @@
       <c r="K6" s="2"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="17"/>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="17"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="19"/>
       <c r="G7" s="4"/>
       <c r="H7" s="5"/>
       <c r="I7" s="6"/>
@@ -785,13 +788,13 @@
       <c r="K7" s="5"/>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="17"/>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="17"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="19"/>
       <c r="G8" s="4"/>
       <c r="H8" s="5"/>
       <c r="I8" s="6"/>
@@ -799,13 +802,13 @@
       <c r="K8" s="5"/>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="17"/>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="17"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="19"/>
       <c r="G9" s="4"/>
       <c r="H9" s="5"/>
       <c r="I9" s="6"/>
@@ -813,13 +816,13 @@
       <c r="K9" s="5"/>
       <c r="L9" s="6"/>
     </row>
-    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="18"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="20"/>
+    <row r="10" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="20"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="22"/>
       <c r="G10" s="7"/>
       <c r="H10" s="8"/>
       <c r="I10" s="9"/>
@@ -827,13 +830,13 @@
       <c r="K10" s="8"/>
       <c r="L10" s="9"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="1" t="s">
         <v>6</v>
       </c>
@@ -844,65 +847,83 @@
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="3"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
+      <c r="M11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N11" s="2"/>
+      <c r="O11" s="3"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
       <c r="G12" s="4"/>
       <c r="H12" s="5"/>
       <c r="I12" s="6"/>
       <c r="J12" s="4"/>
       <c r="K12" s="5"/>
       <c r="L12" s="6"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="6"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="24"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
       <c r="G13" s="4"/>
       <c r="H13" s="5"/>
       <c r="I13" s="6"/>
       <c r="J13" s="4"/>
       <c r="K13" s="5"/>
       <c r="L13" s="6"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="6"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="24"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
       <c r="G14" s="4"/>
       <c r="H14" s="5"/>
       <c r="I14" s="6"/>
       <c r="J14" s="4"/>
       <c r="K14" s="5"/>
       <c r="L14" s="6"/>
-    </row>
-    <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="6"/>
+    </row>
+    <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="24"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
       <c r="G15" s="7"/>
       <c r="H15" s="8"/>
       <c r="I15" s="9"/>
       <c r="J15" s="7"/>
       <c r="K15" s="8"/>
       <c r="L15" s="9"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="M11:O15"/>
     <mergeCell ref="J11:L15"/>
     <mergeCell ref="D1:F5"/>
     <mergeCell ref="A1:C5"/>

</xml_diff>